<commit_message>
Updated resonator source and added status column
</commit_message>
<xml_diff>
--- a/Parts List.xlsx
+++ b/Parts List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="95">
   <si>
     <t>GPS Module</t>
   </si>
@@ -152,9 +152,6 @@
     <t>RESONATOR-16MHZSMD_3.2X1.3</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/murata-electronics-north-america/CSTCE16M0V53-R0/490-1198-1-ND/584635</t>
-  </si>
-  <si>
     <t>DIODE-SCHOTTKY-SS14</t>
   </si>
   <si>
@@ -291,6 +288,27 @@
   </si>
   <si>
     <t>Sourcing from RedBoard</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/murata-electronics/CSTNE16M0V53C000R0/490-17949-1-ND/8747757</t>
+  </si>
+  <si>
+    <t>Bought</t>
+  </si>
+  <si>
+    <t>Cheng</t>
+  </si>
+  <si>
+    <t>Jemmett</t>
+  </si>
+  <si>
+    <t>Jia</t>
+  </si>
+  <si>
+    <t>Liu</t>
+  </si>
+  <si>
+    <t>Ordered</t>
   </si>
 </sst>
 </file>
@@ -457,7 +475,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -502,6 +520,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -520,12 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -848,11 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R80"/>
+  <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W19" sqref="W19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB31" sqref="AB31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,52 +895,58 @@
     <col min="14" max="14" width="3.5546875" customWidth="1"/>
     <col min="15" max="15" width="9.109375" customWidth="1"/>
     <col min="16" max="16" width="3" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="17"/>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="28"/>
+      <c r="G1" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="31"/>
-      <c r="K1" s="25" t="s">
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
+      <c r="K1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25" t="s">
+      <c r="O1" s="28"/>
+      <c r="P1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="25"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="Q1" s="28"/>
+      <c r="S1" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
@@ -934,8 +962,8 @@
       <c r="I2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1" t="s">
         <v>25</v>
@@ -944,8 +972,20 @@
       <c r="Q2" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S2" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="T2" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="U2" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="V2" s="25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="20" t="s">
         <v>5</v>
@@ -975,9 +1015,9 @@
       <c r="P3" s="11"/>
       <c r="Q3" s="11"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1016,10 +1056,13 @@
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
@@ -1058,10 +1101,13 @@
         <f>IF(COUNTA(P5)&gt;0,E5,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>9</v>
@@ -1108,10 +1154,13 @@
         <f t="shared" ref="Q6:Q43" si="4">IF(COUNTA(P6)&gt;0,E6,"")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>12</v>
@@ -1158,10 +1207,13 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>26</v>
@@ -1208,8 +1260,11 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1239,7 +1294,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1269,15 +1324,17 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>30</v>
       </c>
       <c r="E11" s="4">
@@ -1310,16 +1367,21 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="T11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="26" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="4">
@@ -1352,16 +1414,21 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="T12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="4">
@@ -1391,19 +1458,24 @@
         <v>8</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" ref="Q13:Q26" si="9">IF(COUNTA(P13)&gt;0,E13,"")</f>
+        <f t="shared" ref="Q13:Q39" si="9">IF(COUNTA(P13)&gt;0,E13,"")</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="T13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="26" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="4">
@@ -1436,16 +1508,21 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="T14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B15" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="26" t="s">
         <v>38</v>
       </c>
       <c r="E15" s="4">
@@ -1478,16 +1555,21 @@
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="T15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B16" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="26" t="s">
         <v>40</v>
       </c>
       <c r="E16" s="4">
@@ -1520,17 +1602,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="T16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>42</v>
+        <v>84</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>88</v>
       </c>
       <c r="E17" s="4">
         <v>1</v>
@@ -1540,15 +1627,15 @@
         <v>4</v>
       </c>
       <c r="G17" s="6">
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="H17" s="7">
         <f t="shared" si="6"/>
-        <v>0.5</v>
+        <v>0.36</v>
       </c>
       <c r="I17" s="7">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1.44</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="5" t="str">
@@ -1562,17 +1649,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="T17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>44</v>
       </c>
       <c r="E18" s="4">
         <v>1</v>
@@ -1604,17 +1696,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="T18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B19" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>46</v>
       </c>
       <c r="E19" s="4">
         <v>1</v>
@@ -1646,17 +1743,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="T19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>48</v>
       </c>
       <c r="E20" s="4">
         <v>1</v>
@@ -1688,17 +1790,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="T20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="32" t="s">
-        <v>50</v>
       </c>
       <c r="E21" s="4">
         <v>1</v>
@@ -1730,17 +1837,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="T21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>52</v>
       </c>
       <c r="E22" s="4">
         <v>1</v>
@@ -1772,17 +1884,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="T22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>54</v>
       </c>
       <c r="E23" s="4">
         <v>3</v>
@@ -1814,17 +1931,22 @@
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="T23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>55</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>56</v>
       </c>
       <c r="E24" s="4">
         <v>1</v>
@@ -1856,17 +1978,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="T24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="26" t="s">
         <v>57</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>58</v>
       </c>
       <c r="E25" s="4">
         <v>1</v>
@@ -1898,17 +2025,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="T25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B26" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="26" t="s">
         <v>59</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>60</v>
       </c>
       <c r="E26" s="4">
         <v>1</v>
@@ -1940,17 +2072,22 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="T26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="26" t="s">
         <v>61</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="E27" s="4">
         <v>1</v>
@@ -1979,20 +2116,25 @@
         <v>8</v>
       </c>
       <c r="Q27" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28" s="26" t="s">
         <v>63</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>64</v>
       </c>
       <c r="E28" s="4">
         <v>1</v>
@@ -2021,20 +2163,25 @@
         <v>8</v>
       </c>
       <c r="Q28" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B29" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>66</v>
+        <v>84</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>67</v>
       </c>
       <c r="E29" s="4">
         <v>1</v>
@@ -2063,20 +2210,25 @@
         <v>8</v>
       </c>
       <c r="Q29" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="26" t="s">
         <v>67</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>68</v>
       </c>
       <c r="E30" s="4">
         <v>1</v>
@@ -2105,20 +2257,25 @@
         <v>8</v>
       </c>
       <c r="Q30" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B31" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>68</v>
+        <v>84</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>69</v>
       </c>
       <c r="E31" s="4">
         <v>1</v>
@@ -2147,20 +2304,25 @@
         <v>8</v>
       </c>
       <c r="Q31" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B32" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="32" t="s">
-        <v>70</v>
+        <v>84</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>71</v>
       </c>
       <c r="E32" s="4">
         <v>1</v>
@@ -2189,20 +2351,25 @@
         <v>8</v>
       </c>
       <c r="Q32" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B33" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="32" t="s">
-        <v>72</v>
+        <v>84</v>
+      </c>
+      <c r="D33" s="26" t="s">
+        <v>75</v>
       </c>
       <c r="E33" s="4">
         <v>1</v>
@@ -2231,18 +2398,25 @@
         <v>8</v>
       </c>
       <c r="Q33" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B34" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="33" t="s">
-        <v>88</v>
+        <v>78</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="26" t="s">
+        <v>79</v>
       </c>
       <c r="E34" s="4">
         <v>1</v>
@@ -2267,20 +2441,25 @@
       </c>
       <c r="P34" s="4"/>
       <c r="Q34" s="5" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B35" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>74</v>
+        <v>80</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>81</v>
       </c>
       <c r="E35" s="4">
         <v>1</v>
@@ -2309,20 +2488,25 @@
         <v>8</v>
       </c>
       <c r="Q35" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D36" s="26" t="s">
+        <v>73</v>
       </c>
       <c r="E36" s="4">
         <v>1</v>
@@ -2351,20 +2535,25 @@
         <v>8</v>
       </c>
       <c r="Q36" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B37" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="32" t="s">
-        <v>78</v>
+      <c r="D37" s="26" t="s">
+        <v>77</v>
       </c>
       <c r="E37" s="4">
         <v>1</v>
@@ -2393,20 +2582,25 @@
         <v>8</v>
       </c>
       <c r="Q37" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="B38" s="4" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D38" s="32" t="s">
-        <v>80</v>
+      <c r="D38" s="26" t="s">
+        <v>65</v>
       </c>
       <c r="E38" s="4">
         <v>1</v>
@@ -2435,20 +2629,21 @@
         <v>8</v>
       </c>
       <c r="Q38" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="E39" s="4">
         <v>1</v>
@@ -2477,11 +2672,11 @@
         <v>8</v>
       </c>
       <c r="Q39" s="5">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2511,7 +2706,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2541,7 +2736,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2571,7 +2766,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2601,7 +2796,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
@@ -2624,7 +2819,7 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
@@ -2647,7 +2842,7 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
@@ -2670,7 +2865,7 @@
       <c r="P46" s="4"/>
       <c r="Q46" s="4"/>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -2693,7 +2888,7 @@
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
@@ -3348,15 +3543,15 @@
       </c>
       <c r="G76" s="14">
         <f>SUM(G3:G75)</f>
-        <v>149.65999999999997</v>
+        <v>149.51999999999998</v>
       </c>
       <c r="H76" s="14">
         <f t="shared" si="10"/>
-        <v>151.88</v>
+        <v>151.74</v>
       </c>
       <c r="I76" s="14">
         <f t="shared" si="10"/>
-        <v>607.52</v>
+        <v>606.96</v>
       </c>
       <c r="J76" s="16"/>
       <c r="K76" s="15">
@@ -3404,7 +3599,12 @@
       <c r="H80" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <sortState ref="A11:E39">
+    <sortCondition ref="C11:C39"/>
+    <sortCondition ref="A11:A39"/>
+  </sortState>
+  <mergeCells count="10">
+    <mergeCell ref="S1:V1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
@@ -3447,28 +3647,28 @@
     <hyperlink ref="D14" r:id="rId9"/>
     <hyperlink ref="D15" r:id="rId10"/>
     <hyperlink ref="D16" r:id="rId11"/>
-    <hyperlink ref="D17" r:id="rId12"/>
-    <hyperlink ref="D18" r:id="rId13"/>
-    <hyperlink ref="D19" r:id="rId14"/>
-    <hyperlink ref="D20" r:id="rId15"/>
-    <hyperlink ref="D21" r:id="rId16"/>
-    <hyperlink ref="D22" r:id="rId17"/>
-    <hyperlink ref="D23" r:id="rId18"/>
-    <hyperlink ref="D24" r:id="rId19"/>
-    <hyperlink ref="D25" r:id="rId20"/>
-    <hyperlink ref="D26" r:id="rId21"/>
-    <hyperlink ref="D27" r:id="rId22"/>
-    <hyperlink ref="D28" r:id="rId23"/>
+    <hyperlink ref="D18" r:id="rId12"/>
+    <hyperlink ref="D19" r:id="rId13"/>
+    <hyperlink ref="D20" r:id="rId14"/>
+    <hyperlink ref="D21" r:id="rId15"/>
+    <hyperlink ref="D22" r:id="rId16"/>
+    <hyperlink ref="D23" r:id="rId17"/>
+    <hyperlink ref="D24" r:id="rId18"/>
+    <hyperlink ref="D25" r:id="rId19"/>
+    <hyperlink ref="D26" r:id="rId20"/>
+    <hyperlink ref="D27" r:id="rId21"/>
+    <hyperlink ref="D28" r:id="rId22"/>
+    <hyperlink ref="D38" r:id="rId23"/>
     <hyperlink ref="D29" r:id="rId24"/>
     <hyperlink ref="D30" r:id="rId25"/>
     <hyperlink ref="D31" r:id="rId26"/>
     <hyperlink ref="D32" r:id="rId27"/>
-    <hyperlink ref="D33" r:id="rId28"/>
-    <hyperlink ref="D35" r:id="rId29"/>
-    <hyperlink ref="D36" r:id="rId30"/>
-    <hyperlink ref="D37" r:id="rId31"/>
-    <hyperlink ref="D38" r:id="rId32"/>
-    <hyperlink ref="D39" r:id="rId33"/>
+    <hyperlink ref="D36" r:id="rId28"/>
+    <hyperlink ref="D33" r:id="rId29"/>
+    <hyperlink ref="D37" r:id="rId30"/>
+    <hyperlink ref="D34" r:id="rId31"/>
+    <hyperlink ref="D35" r:id="rId32"/>
+    <hyperlink ref="D17" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId34"/>

</xml_diff>